<commit_message>
updated with tuned performance
</commit_message>
<xml_diff>
--- a/Go/results go.xlsx
+++ b/Go/results go.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxkb\OneDrive\Documents\Uni\Year 4\DPT\DPT-coursework\Go\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{6D8AE7A7-A814-452C-9090-8F2205533DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{40F00031-1B5D-4E3B-A072-F98100C35690}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{6D8AE7A7-A814-452C-9090-8F2205533DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2D80AF75-8538-4884-948E-A0E65A059F08}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="42">
   <si>
     <t>dataset</t>
   </si>
@@ -864,34 +864,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>16.229197783</c:v>
+                  <c:v>16.355375959</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.442433862</c:v>
+                  <c:v>9.0661467580000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4784881739999998</c:v>
+                  <c:v>4.7405792340000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1473177049999999</c:v>
+                  <c:v>2.4612415419999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.887656872</c:v>
+                  <c:v>1.6475619239999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2014176399999998</c:v>
+                  <c:v>1.264212785</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6286649900000001</c:v>
+                  <c:v>0.97284453199999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2708245359999999</c:v>
+                  <c:v>0.80052979300000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.98269194800000004</c:v>
+                  <c:v>0.80169590800000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.87803492000000005</c:v>
+                  <c:v>0.80270039400000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -987,34 +987,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>15.18</c:v>
+                  <c:v>15.170999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.667999999999999</c:v>
+                  <c:v>7.5919999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0220000000000002</c:v>
+                  <c:v>3.9729999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9</c:v>
+                  <c:v>2.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7</c:v>
+                  <c:v>1.3759999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2789999999999999</c:v>
+                  <c:v>1.0409999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4319999999999999</c:v>
+                  <c:v>0.79500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>0.64900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.89800000000000002</c:v>
+                  <c:v>0.65100000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.82199999999999995</c:v>
+                  <c:v>0.65300000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1521,34 +1521,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>69.294019246000005</c:v>
+                  <c:v>69.912270863000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.031266256999999</c:v>
+                  <c:v>38.368107610999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.789716234</c:v>
+                  <c:v>20.064803259000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.683234696</c:v>
+                  <c:v>10.406590813999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.311310903000001</c:v>
+                  <c:v>6.9416794399999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.4073229400000002</c:v>
+                  <c:v>5.2270355249999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6996828329999998</c:v>
+                  <c:v>4.0979035460000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3235568109999996</c:v>
+                  <c:v>3.376901384</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.303559549</c:v>
+                  <c:v>3.3745344510000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.8173201890000001</c:v>
+                  <c:v>3.377058415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1644,34 +1644,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>71.704999999999998</c:v>
+                  <c:v>65.084999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.978000000000002</c:v>
+                  <c:v>32.561999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.283999999999999</c:v>
+                  <c:v>17.042000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.716000000000001</c:v>
+                  <c:v>8.8390000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.547000000000001</c:v>
+                  <c:v>5.8940000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.8219999999999992</c:v>
+                  <c:v>4.43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.1849999999999996</c:v>
+                  <c:v>3.399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.8550000000000004</c:v>
+                  <c:v>2.76</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8370000000000002</c:v>
+                  <c:v>2.7610000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4289999999999998</c:v>
+                  <c:v>2.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2160,16 +2160,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>74.895381377000007</c:v>
+                  <c:v>43.908420771999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.819025893000003</c:v>
+                  <c:v>22.003493661</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.332250948999999</c:v>
+                  <c:v>14.206003402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.643024022000001</c:v>
+                  <c:v>14.205709568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2247,16 +2247,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>70.477999999999994</c:v>
+                  <c:v>37.725000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.503999999999998</c:v>
+                  <c:v>18.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.811</c:v>
+                  <c:v>11.741</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.782999999999999</c:v>
+                  <c:v>11.741</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2724,34 +2724,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.98072570344002685</c:v>
+                  <c:v>0.97553996484074335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2792024123680248</c:v>
+                  <c:v>1.7598791762245594</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1282899754171622</c:v>
+                  <c:v>3.3656905834558191</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8377555191422212</c:v>
+                  <c:v>6.482631881401911</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5118707372514999</c:v>
+                  <c:v>9.6842022479271623</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.2300644470169688</c:v>
+                  <c:v>12.620757420990644</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.7726613574471184</c:v>
+                  <c:v>16.400691336773633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.524460270571925</c:v>
+                  <c:v>19.930954509771755</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.19672517353322</c:v>
+                  <c:v>19.901963735606344</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.127287479636912</c:v>
+                  <c:v>19.877058747276507</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2847,34 +2847,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0028138339920949</c:v>
+                  <c:v>1.0029095643003099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3046549537195751</c:v>
+                  <c:v>2.0041018177028449</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1678601538023354</c:v>
+                  <c:v>3.8296352881953184</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.90326</c:v>
+                  <c:v>7.3859907766990283</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.6380422222222215</c:v>
+                  <c:v>11.057515261627907</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6795585783238263</c:v>
+                  <c:v>14.615889529298752</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.63038687150838</c:v>
+                  <c:v>19.138542138364777</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.714156756756756</c:v>
+                  <c:v>23.443976887519259</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.95179732739421</c:v>
+                  <c:v>23.371952380952379</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.51911678832117</c:v>
+                  <c:v>23.300369065849921</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3371,34 +3371,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.98445467874830794</c:v>
+                  <c:v>0.97199037368079022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.286350982558248</c:v>
+                  <c:v>1.7711077900938177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1458770173934485</c:v>
+                  <c:v>3.3867291597050388</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8577117042636355</c:v>
+                  <c:v>6.5299054700585826</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5409876327123735</c:v>
+                  <c:v>9.789281523060362</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.2514595162818978</c:v>
+                  <c:v>13.000495970610416</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.182097146448605</c:v>
+                  <c:v>16.582638785466425</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.814143603209875</c:v>
+                  <c:v>20.123197734755053</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.85125538040975</c:v>
+                  <c:v>20.137312351593472</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.870343088477036</c:v>
+                  <c:v>20.122262019266845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3494,34 +3494,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.91609599051670043</c:v>
+                  <c:v>1.0030219251747716</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1734728464754012</c:v>
+                  <c:v>2.0048425158159819</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0997526850786348</c:v>
+                  <c:v>3.8306350193639243</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9296879038047381</c:v>
+                  <c:v>7.3856411358750993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.6888077422707202</c:v>
+                  <c:v>11.075955548014932</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.4460057810020412</c:v>
+                  <c:v>14.736271331828444</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.620640743734844</c:v>
+                  <c:v>19.206143571638719</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.530105664263646</c:v>
+                  <c:v>23.652783333333335</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.119797498045347</c:v>
+                  <c:v>23.644216588192684</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.15679877515311</c:v>
+                  <c:v>23.652783333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4018,16 +4018,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.9326943478313332</c:v>
+                  <c:v>6.7080673329027105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3969826336655533</c:v>
+                  <c:v>13.386085298902207</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.189026206656926</c:v>
+                  <c:v>20.73353318911165</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.828881334310079</c:v>
+                  <c:v>20.733962046041459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4105,16 +4105,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.9527370243196462</c:v>
+                  <c:v>7.3845195493704443</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.4280343430034135</c:v>
+                  <c:v>14.747538380095289</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.386238047186584</c:v>
+                  <c:v>23.727195298526532</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.844686464181834</c:v>
+                  <c:v>23.727195298526532</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10204,16 +10204,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>545306</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>462756</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>126207</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>18257</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10240,16 +10240,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>130969</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>164306</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>162719</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>132556</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10278,16 +10278,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>178594</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>78581</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>350044</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>2381</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10321,16 +10321,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>490538</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:rowOff>153988</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>319088</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>357188</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>56833</xdr:rowOff>
+      <xdr:rowOff>44133</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10357,16 +10357,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>71120</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10395,16 +10395,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180657</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>53657</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10810,10 +10810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H144" sqref="H144"/>
+    <sheetView topLeftCell="A73" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14902,6 +14902,1109 @@
         <v>22</v>
       </c>
     </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2</v>
+      </c>
+      <c r="D160" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>4</v>
+      </c>
+      <c r="B161" t="s">
+        <v>5</v>
+      </c>
+      <c r="C161">
+        <v>15.955322888</v>
+      </c>
+      <c r="D161" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>4</v>
+      </c>
+      <c r="B162" t="s">
+        <v>5</v>
+      </c>
+      <c r="C162">
+        <v>15.939535336</v>
+      </c>
+      <c r="D162" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>4</v>
+      </c>
+      <c r="B163" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163">
+        <v>15.957351051</v>
+      </c>
+      <c r="D163" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>4</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>16.355375959</v>
+      </c>
+      <c r="D164" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>4</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165">
+        <v>16.372696001000001</v>
+      </c>
+      <c r="D165" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>4</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="C166">
+        <v>16.354559606999999</v>
+      </c>
+      <c r="D166" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>4</v>
+      </c>
+      <c r="B167">
+        <v>2</v>
+      </c>
+      <c r="C167">
+        <v>9.0661467580000004</v>
+      </c>
+      <c r="D167" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>4</v>
+      </c>
+      <c r="B168">
+        <v>2</v>
+      </c>
+      <c r="C168">
+        <v>9.1069415780000007</v>
+      </c>
+      <c r="D168" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>4</v>
+      </c>
+      <c r="B169">
+        <v>2</v>
+      </c>
+      <c r="C169">
+        <v>9.0562717930000005</v>
+      </c>
+      <c r="D169" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>4</v>
+      </c>
+      <c r="B170">
+        <v>4</v>
+      </c>
+      <c r="C170">
+        <v>4.7405792340000001</v>
+      </c>
+      <c r="D170" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>4</v>
+      </c>
+      <c r="B171">
+        <v>4</v>
+      </c>
+      <c r="C171">
+        <v>4.7383210489999996</v>
+      </c>
+      <c r="D171" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>4</v>
+      </c>
+      <c r="B172">
+        <v>4</v>
+      </c>
+      <c r="C172">
+        <v>4.7506756689999996</v>
+      </c>
+      <c r="D172" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>4</v>
+      </c>
+      <c r="B173">
+        <v>8</v>
+      </c>
+      <c r="C173">
+        <v>2.459594939</v>
+      </c>
+      <c r="D173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>4</v>
+      </c>
+      <c r="B174">
+        <v>8</v>
+      </c>
+      <c r="C174">
+        <v>2.4612415419999998</v>
+      </c>
+      <c r="D174" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>4</v>
+      </c>
+      <c r="B175">
+        <v>8</v>
+      </c>
+      <c r="C175">
+        <v>2.4624683790000002</v>
+      </c>
+      <c r="D175" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>4</v>
+      </c>
+      <c r="B176">
+        <v>12</v>
+      </c>
+      <c r="C176">
+        <v>1.655105966</v>
+      </c>
+      <c r="D176" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>4</v>
+      </c>
+      <c r="B177">
+        <v>12</v>
+      </c>
+      <c r="C177">
+        <v>1.6475619239999999</v>
+      </c>
+      <c r="D177" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178">
+        <v>12</v>
+      </c>
+      <c r="C178">
+        <v>1.641362687</v>
+      </c>
+      <c r="D178" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>4</v>
+      </c>
+      <c r="B179">
+        <v>16</v>
+      </c>
+      <c r="C179">
+        <v>1.2778233130000001</v>
+      </c>
+      <c r="D179" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>4</v>
+      </c>
+      <c r="B180">
+        <v>16</v>
+      </c>
+      <c r="C180">
+        <v>1.2413941799999999</v>
+      </c>
+      <c r="D180" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>4</v>
+      </c>
+      <c r="B181">
+        <v>16</v>
+      </c>
+      <c r="C181">
+        <v>1.264212785</v>
+      </c>
+      <c r="D181" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>4</v>
+      </c>
+      <c r="B182">
+        <v>24</v>
+      </c>
+      <c r="C182">
+        <v>0.96828849800000005</v>
+      </c>
+      <c r="D182" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>4</v>
+      </c>
+      <c r="B183">
+        <v>24</v>
+      </c>
+      <c r="C183">
+        <v>0.97327700800000005</v>
+      </c>
+      <c r="D183" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>4</v>
+      </c>
+      <c r="B184">
+        <v>24</v>
+      </c>
+      <c r="C184">
+        <v>0.97284453199999998</v>
+      </c>
+      <c r="D184" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185">
+        <v>32</v>
+      </c>
+      <c r="C185">
+        <v>0.79904500199999995</v>
+      </c>
+      <c r="D185" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>4</v>
+      </c>
+      <c r="B186">
+        <v>32</v>
+      </c>
+      <c r="C186">
+        <v>0.80052979300000005</v>
+      </c>
+      <c r="D186" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>4</v>
+      </c>
+      <c r="B187">
+        <v>32</v>
+      </c>
+      <c r="C187">
+        <v>0.80769802700000004</v>
+      </c>
+      <c r="D187" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>4</v>
+      </c>
+      <c r="B188">
+        <v>48</v>
+      </c>
+      <c r="C188">
+        <v>0.80169590800000001</v>
+      </c>
+      <c r="D188" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189">
+        <v>48</v>
+      </c>
+      <c r="C189">
+        <v>0.79874856599999999</v>
+      </c>
+      <c r="D189" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>4</v>
+      </c>
+      <c r="B190">
+        <v>48</v>
+      </c>
+      <c r="C190">
+        <v>0.80281314299999995</v>
+      </c>
+      <c r="D190" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>4</v>
+      </c>
+      <c r="B191">
+        <v>64</v>
+      </c>
+      <c r="D191" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>4</v>
+      </c>
+      <c r="B192">
+        <v>64</v>
+      </c>
+      <c r="C192">
+        <v>0.80232760700000005</v>
+      </c>
+      <c r="D192" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>4</v>
+      </c>
+      <c r="B193">
+        <v>64</v>
+      </c>
+      <c r="C193">
+        <v>0.80155227900000003</v>
+      </c>
+      <c r="D193" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>8</v>
+      </c>
+      <c r="B194" t="s">
+        <v>5</v>
+      </c>
+      <c r="C194">
+        <v>67.859734355000001</v>
+      </c>
+      <c r="D194" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>8</v>
+      </c>
+      <c r="B195" t="s">
+        <v>5</v>
+      </c>
+      <c r="C195">
+        <v>67.961210575999999</v>
+      </c>
+      <c r="D195" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>8</v>
+      </c>
+      <c r="B196" t="s">
+        <v>5</v>
+      </c>
+      <c r="C196">
+        <v>67.954054280999998</v>
+      </c>
+      <c r="D196" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>8</v>
+      </c>
+      <c r="B197">
+        <v>1</v>
+      </c>
+      <c r="C197">
+        <v>69.912270863000003</v>
+      </c>
+      <c r="D197" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>8</v>
+      </c>
+      <c r="B198">
+        <v>1</v>
+      </c>
+      <c r="C198">
+        <v>69.762976769000005</v>
+      </c>
+      <c r="D198" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>8</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+      <c r="C199">
+        <v>69.918605012</v>
+      </c>
+      <c r="D199" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>8</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+      <c r="C200">
+        <v>38.368107610999999</v>
+      </c>
+      <c r="D200" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>8</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201">
+        <v>38.354777241999997</v>
+      </c>
+      <c r="D201" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>8</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202">
+        <v>38.372485050000002</v>
+      </c>
+      <c r="D202" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>8</v>
+      </c>
+      <c r="B203">
+        <v>4</v>
+      </c>
+      <c r="C203">
+        <v>20.064803259000001</v>
+      </c>
+      <c r="D203" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>8</v>
+      </c>
+      <c r="B204">
+        <v>4</v>
+      </c>
+      <c r="C204">
+        <v>20.091608399999998</v>
+      </c>
+      <c r="D204" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>8</v>
+      </c>
+      <c r="B205">
+        <v>4</v>
+      </c>
+      <c r="C205">
+        <v>19.994704351999999</v>
+      </c>
+      <c r="D205" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>8</v>
+      </c>
+      <c r="B206">
+        <v>8</v>
+      </c>
+      <c r="C206">
+        <v>10.399656049000001</v>
+      </c>
+      <c r="D206" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>8</v>
+      </c>
+      <c r="B207">
+        <v>8</v>
+      </c>
+      <c r="C207">
+        <v>10.41666114</v>
+      </c>
+      <c r="D207" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>8</v>
+      </c>
+      <c r="B208">
+        <v>8</v>
+      </c>
+      <c r="C208">
+        <v>10.406590813999999</v>
+      </c>
+      <c r="D208" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>8</v>
+      </c>
+      <c r="B209">
+        <v>12</v>
+      </c>
+      <c r="C209">
+        <v>6.9373853380000003</v>
+      </c>
+      <c r="D209" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>8</v>
+      </c>
+      <c r="B210">
+        <v>12</v>
+      </c>
+      <c r="C210">
+        <v>6.9448872780000004</v>
+      </c>
+      <c r="D210" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>8</v>
+      </c>
+      <c r="B211">
+        <v>12</v>
+      </c>
+      <c r="C211">
+        <v>6.9416794399999997</v>
+      </c>
+      <c r="D211" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>8</v>
+      </c>
+      <c r="B212">
+        <v>16</v>
+      </c>
+      <c r="C212">
+        <v>5.2417380800000002</v>
+      </c>
+      <c r="D212" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>8</v>
+      </c>
+      <c r="B213">
+        <v>16</v>
+      </c>
+      <c r="C213">
+        <v>5.2270355249999998</v>
+      </c>
+      <c r="D213" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>8</v>
+      </c>
+      <c r="B214">
+        <v>16</v>
+      </c>
+      <c r="C214">
+        <v>5.2265507170000003</v>
+      </c>
+      <c r="D214" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>8</v>
+      </c>
+      <c r="B215">
+        <v>24</v>
+      </c>
+      <c r="C215">
+        <v>4.0995703380000004</v>
+      </c>
+      <c r="D215" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>8</v>
+      </c>
+      <c r="B216">
+        <v>24</v>
+      </c>
+      <c r="C216">
+        <v>4.0914943319999999</v>
+      </c>
+      <c r="D216" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>8</v>
+      </c>
+      <c r="B217">
+        <v>24</v>
+      </c>
+      <c r="C217">
+        <v>4.0979035460000004</v>
+      </c>
+      <c r="D217" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>8</v>
+      </c>
+      <c r="B218">
+        <v>32</v>
+      </c>
+      <c r="C218">
+        <v>3.3771433709999998</v>
+      </c>
+      <c r="D218" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>8</v>
+      </c>
+      <c r="B219">
+        <v>32</v>
+      </c>
+      <c r="C219">
+        <v>3.376303375</v>
+      </c>
+      <c r="D219" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>8</v>
+      </c>
+      <c r="B220">
+        <v>32</v>
+      </c>
+      <c r="C220">
+        <v>3.376901384</v>
+      </c>
+      <c r="D220" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>8</v>
+      </c>
+      <c r="B221">
+        <v>48</v>
+      </c>
+      <c r="C221">
+        <v>3.3745344510000002</v>
+      </c>
+      <c r="D221" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>8</v>
+      </c>
+      <c r="B222">
+        <v>48</v>
+      </c>
+      <c r="C222">
+        <v>3.3812914329999999</v>
+      </c>
+      <c r="D222" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>8</v>
+      </c>
+      <c r="B223">
+        <v>48</v>
+      </c>
+      <c r="C223">
+        <v>3.3747480200000002</v>
+      </c>
+      <c r="D223" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>8</v>
+      </c>
+      <c r="B224">
+        <v>64</v>
+      </c>
+      <c r="C224">
+        <v>3.3769939</v>
+      </c>
+      <c r="D224" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>8</v>
+      </c>
+      <c r="B225">
+        <v>64</v>
+      </c>
+      <c r="C225">
+        <v>3.3809063610000001</v>
+      </c>
+      <c r="D225" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>8</v>
+      </c>
+      <c r="B226">
+        <v>64</v>
+      </c>
+      <c r="C226">
+        <v>3.377058415</v>
+      </c>
+      <c r="D226" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>11</v>
+      </c>
+      <c r="B227">
+        <v>8</v>
+      </c>
+      <c r="C227">
+        <v>43.908420771999999</v>
+      </c>
+      <c r="D227" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>11</v>
+      </c>
+      <c r="B228">
+        <v>8</v>
+      </c>
+      <c r="C228">
+        <v>43.906616341000003</v>
+      </c>
+      <c r="D228" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>11</v>
+      </c>
+      <c r="B229">
+        <v>8</v>
+      </c>
+      <c r="C229">
+        <v>43.911602608999999</v>
+      </c>
+      <c r="D229" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>11</v>
+      </c>
+      <c r="B230">
+        <v>16</v>
+      </c>
+      <c r="C230">
+        <v>22.039932286999999</v>
+      </c>
+      <c r="D230" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>11</v>
+      </c>
+      <c r="B231">
+        <v>16</v>
+      </c>
+      <c r="C231">
+        <v>21.989646441000001</v>
+      </c>
+      <c r="D231" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>11</v>
+      </c>
+      <c r="B232">
+        <v>16</v>
+      </c>
+      <c r="C232">
+        <v>22.003493661</v>
+      </c>
+      <c r="D232" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>11</v>
+      </c>
+      <c r="B233">
+        <v>32</v>
+      </c>
+      <c r="C233">
+        <v>14.213648824</v>
+      </c>
+      <c r="D233" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>11</v>
+      </c>
+      <c r="B234">
+        <v>32</v>
+      </c>
+      <c r="C234">
+        <v>14.205969226000001</v>
+      </c>
+      <c r="D234" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>11</v>
+      </c>
+      <c r="B235">
+        <v>32</v>
+      </c>
+      <c r="C235">
+        <v>14.206003402</v>
+      </c>
+      <c r="D235" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>11</v>
+      </c>
+      <c r="B236">
+        <v>64</v>
+      </c>
+      <c r="C236">
+        <v>14.198845107</v>
+      </c>
+      <c r="D236" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>11</v>
+      </c>
+      <c r="B237">
+        <v>64</v>
+      </c>
+      <c r="C237">
+        <v>14.205873413999999</v>
+      </c>
+      <c r="D237" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>11</v>
+      </c>
+      <c r="B238">
+        <v>64</v>
+      </c>
+      <c r="C238">
+        <v>14.205709568</v>
+      </c>
+      <c r="D238" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14912,7 +16015,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G12"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14962,28 +16065,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>16.229197783</v>
+        <v>16.355375959</v>
       </c>
       <c r="C3">
-        <v>15.18</v>
+        <v>15.170999999999999</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>69.294019246000005</v>
+        <v>69.912270863000003</v>
       </c>
       <c r="G3">
-        <v>71.704999999999998</v>
+        <v>65.084999999999994</v>
       </c>
       <c r="I3">
         <v>8</v>
       </c>
       <c r="J3">
-        <v>74.895381377000007</v>
+        <v>43.908420771999999</v>
       </c>
       <c r="K3">
-        <v>70.477999999999994</v>
+        <v>37.725000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -14991,28 +16094,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>12.442433862</v>
+        <v>9.0661467580000004</v>
       </c>
       <c r="C4">
-        <v>11.667999999999999</v>
+        <v>7.5919999999999996</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>53.031266256999999</v>
+        <v>38.368107610999999</v>
       </c>
       <c r="G4">
-        <v>55.978000000000002</v>
+        <v>32.561999999999998</v>
       </c>
       <c r="I4">
         <v>16</v>
       </c>
       <c r="J4">
-        <v>39.819025893000003</v>
+        <v>22.003493661</v>
       </c>
       <c r="K4">
-        <v>37.503999999999998</v>
+        <v>18.89</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -15020,28 +16123,28 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7.4784881739999998</v>
+        <v>4.7405792340000001</v>
       </c>
       <c r="C5">
-        <v>7.0220000000000002</v>
+        <v>3.9729999999999999</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
-        <v>31.789716234</v>
+        <v>20.064803259000001</v>
       </c>
       <c r="G5">
-        <v>31.283999999999999</v>
+        <v>17.042000000000002</v>
       </c>
       <c r="I5">
         <v>32</v>
       </c>
       <c r="J5">
-        <v>22.332250948999999</v>
+        <v>14.206003402</v>
       </c>
       <c r="K5">
-        <v>20.811</v>
+        <v>11.741</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -15049,28 +16152,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>4.1473177049999999</v>
+        <v>2.4612415419999998</v>
       </c>
       <c r="C6">
-        <v>3.9</v>
+        <v>2.06</v>
       </c>
       <c r="E6">
         <v>8</v>
       </c>
       <c r="F6">
-        <v>17.683234696</v>
+        <v>10.406590813999999</v>
       </c>
       <c r="G6">
-        <v>16.716000000000001</v>
+        <v>8.8390000000000004</v>
       </c>
       <c r="I6">
         <v>64</v>
       </c>
       <c r="J6">
-        <v>15.643024022000001</v>
+        <v>14.205709568</v>
       </c>
       <c r="K6">
-        <v>14.782999999999999</v>
+        <v>11.741</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -15078,19 +16181,19 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>2.887656872</v>
+        <v>1.6475619239999999</v>
       </c>
       <c r="C7">
-        <v>2.7</v>
+        <v>1.3759999999999999</v>
       </c>
       <c r="E7">
         <v>12</v>
       </c>
       <c r="F7">
-        <v>12.311310903000001</v>
+        <v>6.9416794399999997</v>
       </c>
       <c r="G7">
-        <v>11.547000000000001</v>
+        <v>5.8940000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -15098,19 +16201,19 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>2.2014176399999998</v>
+        <v>1.264212785</v>
       </c>
       <c r="C8">
-        <v>2.2789999999999999</v>
+        <v>1.0409999999999999</v>
       </c>
       <c r="E8">
         <v>16</v>
       </c>
       <c r="F8">
-        <v>9.4073229400000002</v>
+        <v>5.2270355249999998</v>
       </c>
       <c r="G8">
-        <v>8.8219999999999992</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -15118,19 +16221,19 @@
         <v>24</v>
       </c>
       <c r="B9">
-        <v>1.6286649900000001</v>
+        <v>0.97284453199999998</v>
       </c>
       <c r="C9">
-        <v>1.4319999999999999</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="E9">
         <v>24</v>
       </c>
       <c r="F9">
-        <v>6.6996828329999998</v>
+        <v>4.0979035460000004</v>
       </c>
       <c r="G9">
-        <v>6.1849999999999996</v>
+        <v>3.399</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -15138,19 +16241,19 @@
         <v>32</v>
       </c>
       <c r="B10">
-        <v>1.2708245359999999</v>
+        <v>0.80052979300000005</v>
       </c>
       <c r="C10">
-        <v>1.1100000000000001</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="E10">
         <v>32</v>
       </c>
       <c r="F10">
-        <v>5.3235568109999996</v>
+        <v>3.376901384</v>
       </c>
       <c r="G10">
-        <v>4.8550000000000004</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -15158,19 +16261,19 @@
         <v>48</v>
       </c>
       <c r="B11">
-        <v>0.98269194800000004</v>
+        <v>0.80169590800000001</v>
       </c>
       <c r="C11">
-        <v>0.89800000000000002</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="E11">
         <v>48</v>
       </c>
       <c r="F11">
-        <v>4.303559549</v>
+        <v>3.3745344510000002</v>
       </c>
       <c r="G11">
-        <v>3.8370000000000002</v>
+        <v>2.7610000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -15178,19 +16281,19 @@
         <v>64</v>
       </c>
       <c r="B12">
-        <v>0.87803492000000005</v>
+        <v>0.80270039400000004</v>
       </c>
       <c r="C12">
-        <v>0.82199999999999995</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="E12">
         <v>64</v>
       </c>
       <c r="F12">
-        <v>3.8173201890000001</v>
+        <v>3.377058415</v>
       </c>
       <c r="G12">
-        <v>3.4289999999999998</v>
+        <v>2.76</v>
       </c>
     </row>
   </sheetData>
@@ -15204,7 +16307,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15228,7 +16331,7 @@
         <v>29</v>
       </c>
       <c r="B2">
-        <v>15.916391411999999</v>
+        <v>15.955322888</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
@@ -15263,40 +16366,40 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>15.222714</v>
+        <v>15.215140999999999</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
         <f>$B$2 / Graphs!B3</f>
-        <v>0.98072570344002685</v>
+        <v>0.97553996484074335</v>
       </c>
       <c r="F3">
         <f>$B$3 / Graphs!C3</f>
-        <v>1.0028138339920949</v>
+        <v>1.0029095643003099</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
         <f>$B$6 / Graphs!F3</f>
-        <v>0.98445467874830794</v>
+        <v>0.97199037368079022</v>
       </c>
       <c r="J3">
         <f>$B$7 / Graphs!G3</f>
-        <v>0.91609599051670043</v>
+        <v>1.0030219251747716</v>
       </c>
       <c r="L3">
         <v>8</v>
       </c>
       <c r="M3">
         <f>$B$10 / Graphs!J3</f>
-        <v>3.9326943478313332</v>
+        <v>6.7080673329027105</v>
       </c>
       <c r="N3">
         <f>$B$11 / Graphs!K3</f>
-        <v>3.9527370243196462</v>
+        <v>7.3845195493704443</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -15305,33 +16408,33 @@
       </c>
       <c r="E4">
         <f>$B$2 / Graphs!B4</f>
-        <v>1.2792024123680248</v>
+        <v>1.7598791762245594</v>
       </c>
       <c r="F4">
         <f>$B$3 / Graphs!C4</f>
-        <v>1.3046549537195751</v>
+        <v>2.0041018177028449</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4">
         <f>$B$6 / Graphs!F4</f>
-        <v>1.286350982558248</v>
+        <v>1.7711077900938177</v>
       </c>
       <c r="J4">
         <f>$B$7 / Graphs!G4</f>
-        <v>1.1734728464754012</v>
+        <v>2.0048425158159819</v>
       </c>
       <c r="L4">
         <v>16</v>
       </c>
       <c r="M4">
         <f>$B$10 / Graphs!J4</f>
-        <v>7.3969826336655533</v>
+        <v>13.386085298902207</v>
       </c>
       <c r="N4">
         <f>$B$11 / Graphs!K4</f>
-        <v>7.4280343430034135</v>
+        <v>14.747538380095289</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -15343,33 +16446,33 @@
       </c>
       <c r="E5">
         <f>$B$2 / Graphs!B5</f>
-        <v>2.1282899754171622</v>
+        <v>3.3656905834558191</v>
       </c>
       <c r="F5">
         <f>$B$3 / Graphs!C5</f>
-        <v>2.1678601538023354</v>
+        <v>3.8296352881953184</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="I5">
         <f>$B$6 / Graphs!F5</f>
-        <v>2.1458770173934485</v>
+        <v>3.3867291597050388</v>
       </c>
       <c r="J5">
         <f>$B$7 / Graphs!G5</f>
-        <v>2.0997526850786348</v>
+        <v>3.8306350193639243</v>
       </c>
       <c r="L5">
         <v>32</v>
       </c>
       <c r="M5">
         <f>$B$10 / Graphs!J5</f>
-        <v>13.189026206656926</v>
+        <v>20.73353318911165</v>
       </c>
       <c r="N5">
         <f>$B$11 / Graphs!K5</f>
-        <v>13.386238047186584</v>
+        <v>23.727195298526532</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -15377,40 +16480,40 @@
         <v>29</v>
       </c>
       <c r="B6">
-        <v>68.216821456000005</v>
+        <v>67.954054280999998</v>
       </c>
       <c r="D6">
         <v>8</v>
       </c>
       <c r="E6">
         <f>$B$2 / Graphs!B6</f>
-        <v>3.8377555191422212</v>
+        <v>6.482631881401911</v>
       </c>
       <c r="F6">
         <f>$B$3 / Graphs!C6</f>
-        <v>3.90326</v>
+        <v>7.3859907766990283</v>
       </c>
       <c r="H6">
         <v>8</v>
       </c>
       <c r="I6">
         <f>$B$6 / Graphs!F6</f>
-        <v>3.8577117042636355</v>
+        <v>6.5299054700585826</v>
       </c>
       <c r="J6">
         <f>$B$7 / Graphs!G6</f>
-        <v>3.9296879038047381</v>
+        <v>7.3856411358750993</v>
       </c>
       <c r="L6">
         <v>64</v>
       </c>
       <c r="M6">
         <f>$B$10 / Graphs!J6</f>
-        <v>18.828881334310079</v>
+        <v>20.733962046041459</v>
       </c>
       <c r="N6">
         <f>$B$11 / Graphs!K6</f>
-        <v>18.844686464181834</v>
+        <v>23.727195298526532</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -15418,29 +16521,29 @@
         <v>30</v>
       </c>
       <c r="B7">
-        <v>65.688663000000005</v>
+        <v>65.281682000000004</v>
       </c>
       <c r="D7">
         <v>12</v>
       </c>
       <c r="E7">
         <f>$B$2 / Graphs!B7</f>
-        <v>5.5118707372514999</v>
+        <v>9.6842022479271623</v>
       </c>
       <c r="F7">
         <f>$B$3 / Graphs!C7</f>
-        <v>5.6380422222222215</v>
+        <v>11.057515261627907</v>
       </c>
       <c r="H7">
         <v>12</v>
       </c>
       <c r="I7">
         <f>$B$6 / Graphs!F7</f>
-        <v>5.5409876327123735</v>
+        <v>9.789281523060362</v>
       </c>
       <c r="J7">
         <f>$B$7 / Graphs!G7</f>
-        <v>5.6888077422707202</v>
+        <v>11.075955548014932</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -15449,22 +16552,22 @@
       </c>
       <c r="E8">
         <f>$B$2 / Graphs!B8</f>
-        <v>7.2300644470169688</v>
+        <v>12.620757420990644</v>
       </c>
       <c r="F8">
         <f>$B$3 / Graphs!C8</f>
-        <v>6.6795585783238263</v>
+        <v>14.615889529298752</v>
       </c>
       <c r="H8">
         <v>16</v>
       </c>
       <c r="I8">
         <f>$B$6 / Graphs!F8</f>
-        <v>7.2514595162818978</v>
+        <v>13.000495970610416</v>
       </c>
       <c r="J8">
         <f>$B$7 / Graphs!G8</f>
-        <v>7.4460057810020412</v>
+        <v>14.736271331828444</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -15476,22 +16579,22 @@
       </c>
       <c r="E9">
         <f>$B$2 / Graphs!B9</f>
-        <v>9.7726613574471184</v>
+        <v>16.400691336773633</v>
       </c>
       <c r="F9">
         <f>$B$3 / Graphs!C9</f>
-        <v>10.63038687150838</v>
+        <v>19.138542138364777</v>
       </c>
       <c r="H9">
         <v>24</v>
       </c>
       <c r="I9">
         <f>$B$6 / Graphs!F9</f>
-        <v>10.182097146448605</v>
+        <v>16.582638785466425</v>
       </c>
       <c r="J9">
         <f>$B$7 / Graphs!G9</f>
-        <v>10.620640743734844</v>
+        <v>19.206143571638719</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -15506,22 +16609,22 @@
       </c>
       <c r="E10">
         <f>$B$2 / Graphs!B10</f>
-        <v>12.524460270571925</v>
+        <v>19.930954509771755</v>
       </c>
       <c r="F10">
         <f>$B$3 / Graphs!C10</f>
-        <v>13.714156756756756</v>
+        <v>23.443976887519259</v>
       </c>
       <c r="H10">
         <v>32</v>
       </c>
       <c r="I10">
         <f>$B$6 / Graphs!F10</f>
-        <v>12.814143603209875</v>
+        <v>20.123197734755053</v>
       </c>
       <c r="J10">
         <f>$B$7 / Graphs!G10</f>
-        <v>13.530105664263646</v>
+        <v>23.652783333333335</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -15536,22 +16639,22 @@
       </c>
       <c r="E11">
         <f>$B$2 / Graphs!B11</f>
-        <v>16.19672517353322</v>
+        <v>19.901963735606344</v>
       </c>
       <c r="F11">
         <f>$B$3 / Graphs!C11</f>
-        <v>16.95179732739421</v>
+        <v>23.371952380952379</v>
       </c>
       <c r="H11">
         <v>48</v>
       </c>
       <c r="I11">
         <f>$B$6 / Graphs!F11</f>
-        <v>15.85125538040975</v>
+        <v>20.137312351593472</v>
       </c>
       <c r="J11">
         <f>$B$7 / Graphs!G11</f>
-        <v>17.119797498045347</v>
+        <v>23.644216588192684</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -15560,22 +16663,22 @@
       </c>
       <c r="E12">
         <f>$B$2 / Graphs!B12</f>
-        <v>18.127287479636912</v>
+        <v>19.877058747276507</v>
       </c>
       <c r="F12">
         <f>$B$3 / Graphs!C12</f>
-        <v>18.51911678832117</v>
+        <v>23.300369065849921</v>
       </c>
       <c r="H12">
         <v>64</v>
       </c>
       <c r="I12">
         <f>$B$6 / Graphs!F12</f>
-        <v>17.870343088477036</v>
+        <v>20.122262019266845</v>
       </c>
       <c r="J12">
         <f>$B$7 / Graphs!G12</f>
-        <v>19.15679877515311</v>
+        <v>23.652783333333335</v>
       </c>
     </row>
   </sheetData>
@@ -15589,7 +16692,7 @@
   <dimension ref="B1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+      <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Final tweaks for pt1
</commit_message>
<xml_diff>
--- a/Go/results go.xlsx
+++ b/Go/results go.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxkb\OneDrive\Documents\Uni\Year 4\DPT\DPT-coursework\Go\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{6D8AE7A7-A814-452C-9090-8F2205533DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2D80AF75-8538-4884-948E-A0E65A059F08}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{6D8AE7A7-A814-452C-9090-8F2205533DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99F4678E-8D02-48A4-8386-5CB7485DF18A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4583,10 +4583,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Performance Tuning'!$C$3:$C$12</c:f>
+              <c:f>'Performance Tuning'!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>69.294019246000005</c:v>
                 </c:pt>
@@ -4610,22 +4610,16 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>5.3235568109999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.303559549</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.8173201890000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Performance Tuning'!$B$3:$B$12</c:f>
+              <c:f>'Performance Tuning'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4649,12 +4643,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4706,10 +4694,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Performance Tuning'!$D$3:$D$12</c:f>
+              <c:f>'Performance Tuning'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>76.918487597999999</c:v>
                 </c:pt>
@@ -4733,22 +4721,16 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.3952723389999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.388085486</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.3845105489999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Performance Tuning'!$B$3:$B$12</c:f>
+              <c:f>'Performance Tuning'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4772,12 +4754,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5225,10 +5201,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Performance Tuning'!$C$16:$C$25</c:f>
+              <c:f>'Performance Tuning'!$C$16:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>71.704999999999998</c:v>
                 </c:pt>
@@ -5252,22 +5228,16 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4.8550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.8370000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.4289999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Performance Tuning'!$B$16:$B$25</c:f>
+              <c:f>'Performance Tuning'!$B$16:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5291,12 +5261,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5348,10 +5312,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Performance Tuning'!$D$16:$D$25</c:f>
+              <c:f>'Performance Tuning'!$D$16:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>65.084999999999994</c:v>
                 </c:pt>
@@ -5374,12 +5338,6 @@
                   <c:v>3.399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.76</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.7610000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>2.76</c:v>
                 </c:pt>
               </c:numCache>
@@ -5387,10 +5345,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Performance Tuning'!$B$16:$B$25</c:f>
+              <c:f>'Performance Tuning'!$B$16:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5414,12 +5372,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>

</xml_diff>

<commit_message>
Final report, and workbooks updated with erlang metrics
</commit_message>
<xml_diff>
--- a/Go/results go.xlsx
+++ b/Go/results go.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxkb\OneDrive\Documents\Uni\Year 4\DPT\DPT-coursework\Go\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{6D8AE7A7-A814-452C-9090-8F2205533DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99F4678E-8D02-48A4-8386-5CB7485DF18A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7685401B-2C3A-493F-AD69-4CD0E71F5802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7660" yWindow="5610" windowWidth="28800" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results go" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="45">
   <si>
     <t>dataset</t>
   </si>
@@ -158,12 +158,21 @@
   <si>
     <t>OpenMP DS2</t>
   </si>
+  <si>
+    <t>Erlang</t>
+  </si>
+  <si>
+    <t>Sequential Erlang</t>
+  </si>
+  <si>
+    <t>Ideal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +303,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -640,8 +656,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -739,7 +756,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Go vs OpenMP Execution Time</a:t>
+              <a:t> Go vs OpenMP vs Erlang Execution Time</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -820,6 +837,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>16.355375959</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0661467580000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7405792340000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4612415419999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6475619239999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.264212785</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97284453199999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.80052979300000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.80169590800000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.80270039400000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -853,45 +909,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$B$3:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>16.355375959</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.0661467580000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.7405792340000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.4612415419999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6475619239999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.264212785</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.97284453199999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.80052979300000005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.80169590800000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.80270039400000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -943,6 +960,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15.170999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5919999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9729999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3759999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0409999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.65100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65300000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -976,45 +1032,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$C$3:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>15.170999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.5919999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.9729999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.06</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.3759999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0409999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.79500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.64900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.65100000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.65300000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1023,6 +1040,129 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-39D5-4B8F-9CE3-4232313EA1E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Erlang</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Graphs!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>27.643243999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.842316</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.903312</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6745109999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1556680000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8414100000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7114829999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.310508</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1547100000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8771610000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-14EE-46E7-BE4A-DE97E8EE8217}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1081,7 +1221,7 @@
                   <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Number of Threads</a:t>
+                  <a:t>Median Runtime(s)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="1000">
                   <a:effectLst/>
@@ -1201,13 +1341,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Median</a:t>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Runtime (s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1396,7 +1531,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Go vs OpenMP Execution Time</a:t>
+              <a:t> Go vs OpenMP vs Erlang Execution Time</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1477,6 +1612,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>69.912270863000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.368107610999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.064803259000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.406590813999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9416794399999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2270355249999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0979035460000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.376901384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3745344510000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.377058415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1510,45 +1684,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$F$3:$F$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>69.912270863000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>38.368107610999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.064803259000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.406590813999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.9416794399999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.2270355249999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.0979035460000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.376901384</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.3745344510000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.377058415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1600,6 +1735,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>65.084999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.561999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.042000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.8390000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7610000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1633,45 +1807,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$G$3:$G$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>65.084999999999994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32.561999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17.042000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.8390000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.8940000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.43</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.399</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.76</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.7610000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1680,6 +1815,129 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9412-4402-8044-17A977A41EBB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Erlang</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Graphs!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>117.767549</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.972942000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.275478999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.341128000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.141628999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.746213999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.129220999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5707269999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.9244919999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.1972329999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-69A9-42CC-A2D1-533ECBDE1199}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1738,7 +1996,7 @@
                   <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Number of Threads</a:t>
+                  <a:t>Median Runtime (s)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="1000">
                   <a:effectLst/>
@@ -1858,11 +2116,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Median</a:t>
+                  <a:t>Number of</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Runtime (s)</a:t>
+                  <a:t> Threads</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -2053,7 +2311,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Go vs OpenMP Execution Time</a:t>
+              <a:t> Go vs OpenMP vs Erlang Execution Time</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2134,6 +2392,27 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$J$3:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>43.908420771999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.003493661</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.206003402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.205709568</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$I$3:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2149,27 +2428,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$J$3:$J$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>43.908420771999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22.003493661</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.206003402</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.205709568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2221,6 +2479,27 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$K$3:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>37.725000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.741</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.741</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$I$3:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2236,27 +2515,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$K$3:$K$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>37.725000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.89</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.741</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.741</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2265,6 +2523,93 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-202D-4DB5-875F-7C762392A130}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Erlang</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Graphs!$L$3:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>129.50238899999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.370891999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.371085999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.137900000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-89AE-4AAF-B861-342326B177F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2323,7 +2668,7 @@
                   <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Number of Threads</a:t>
+                  <a:t>Median Runtime (s)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="1000">
                   <a:effectLst/>
@@ -2443,13 +2788,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Median</a:t>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Runtime (s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2638,7 +2978,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> vs C+OpenMP Absolute Speedup</a:t>
+              <a:t> vs C+OpenMP vs Erlang Absolute Speedup</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2922,6 +3262,240 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EE25-4E92-84EE-126591579FF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedups!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Erlang</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Speedups!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99699991795463661</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2617852429202105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1359099121217873</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5911489344402532</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3456335823020407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1745301855308332</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.164294594507878</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.928247813900667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.790729146845747</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.681911674065249</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Speedups!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9992-4B0E-861D-676651A3D184}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedups!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Speedups!$A$16:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Speedups!$A$16:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9992-4B0E-861D-676651A3D184}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3572,6 +4146,240 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedups!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Erlang</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Speedups!$K$3:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0094327428008203</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3212685653871361</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1124372837412899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7930485463063102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.6229545982478459</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0988236505278159</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8009938148542286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.421043876813121</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.001393149239094</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.517239333504975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Speedups!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6809-410B-9901-E897EA9F8296}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedups!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Speedups!$A$16:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Speedups!$A$16:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6809-410B-9901-E897EA9F8296}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -4144,6 +4952,180 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-03AA-4F03-B1A4-73F2007B51A4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedups!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Erlang</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Speedups!$O$3:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.8296174443546369</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1491744404843462</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.704788685378515</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.431767725955957</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Speedups!$L$3:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-562B-458B-9D35-624E0F590711}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedups!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Speedups!$A$16,Speedups!$A$19,Speedups!$A$21,Speedups!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Speedups!$A$16,Speedups!$A$19,Speedups!$A$21,Speedups!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-562B-458B-9D35-624E0F590711}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15964,15 +16946,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2401614-BA96-48EB-BC57-655DFAADC499}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y37" sqref="Y37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -15983,7 +16965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -15993,6 +16975,9 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
       <c r="E2" t="s">
         <v>25</v>
       </c>
@@ -16002,6 +16987,9 @@
       <c r="G2" t="s">
         <v>24</v>
       </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
       <c r="I2" t="s">
         <v>25</v>
       </c>
@@ -16011,8 +16999,11 @@
       <c r="K2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -16022,6 +17013,9 @@
       <c r="C3">
         <v>15.170999999999999</v>
       </c>
+      <c r="D3">
+        <v>27.643243999999999</v>
+      </c>
       <c r="E3">
         <v>1</v>
       </c>
@@ -16031,6 +17025,9 @@
       <c r="G3">
         <v>65.084999999999994</v>
       </c>
+      <c r="H3">
+        <v>117.767549</v>
+      </c>
       <c r="I3">
         <v>8</v>
       </c>
@@ -16040,8 +17037,11 @@
       <c r="K3">
         <v>37.725000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>129.50238899999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -16051,6 +17051,9 @@
       <c r="C4">
         <v>7.5919999999999996</v>
       </c>
+      <c r="D4">
+        <v>21.842316</v>
+      </c>
       <c r="E4">
         <v>2</v>
       </c>
@@ -16060,6 +17063,9 @@
       <c r="G4">
         <v>32.561999999999998</v>
       </c>
+      <c r="H4">
+        <v>89.972942000000003</v>
+      </c>
       <c r="I4">
         <v>16</v>
       </c>
@@ -16069,8 +17075,11 @@
       <c r="K4">
         <v>18.89</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>69.370891999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -16080,6 +17089,9 @@
       <c r="C5">
         <v>3.9729999999999999</v>
       </c>
+      <c r="D5">
+        <v>12.903312</v>
+      </c>
       <c r="E5">
         <v>4</v>
       </c>
@@ -16089,6 +17101,9 @@
       <c r="G5">
         <v>17.042000000000002</v>
       </c>
+      <c r="H5">
+        <v>56.275478999999997</v>
+      </c>
       <c r="I5">
         <v>32</v>
       </c>
@@ -16098,8 +17113,11 @@
       <c r="K5">
         <v>11.741</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>42.371085999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>8</v>
       </c>
@@ -16109,6 +17127,9 @@
       <c r="C6">
         <v>2.06</v>
       </c>
+      <c r="D6">
+        <v>7.6745109999999999</v>
+      </c>
       <c r="E6">
         <v>8</v>
       </c>
@@ -16118,6 +17139,9 @@
       <c r="G6">
         <v>8.8390000000000004</v>
       </c>
+      <c r="H6">
+        <v>31.341128000000001</v>
+      </c>
       <c r="I6">
         <v>64</v>
       </c>
@@ -16127,8 +17151,11 @@
       <c r="K6">
         <v>11.741</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>32.137900000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>12</v>
       </c>
@@ -16138,6 +17165,9 @@
       <c r="C7">
         <v>1.3759999999999999</v>
       </c>
+      <c r="D7">
+        <v>5.1556680000000004</v>
+      </c>
       <c r="E7">
         <v>12</v>
       </c>
@@ -16147,8 +17177,11 @@
       <c r="G7">
         <v>5.8940000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>21.141628999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>16</v>
       </c>
@@ -16158,6 +17191,9 @@
       <c r="C8">
         <v>1.0409999999999999</v>
       </c>
+      <c r="D8">
+        <v>3.8414100000000002</v>
+      </c>
       <c r="E8">
         <v>16</v>
       </c>
@@ -16167,8 +17203,11 @@
       <c r="G8">
         <v>4.43</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>16.746213999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>24</v>
       </c>
@@ -16178,6 +17217,9 @@
       <c r="C9">
         <v>0.79500000000000004</v>
       </c>
+      <c r="D9">
+        <v>2.7114829999999999</v>
+      </c>
       <c r="E9">
         <v>24</v>
       </c>
@@ -16187,8 +17229,11 @@
       <c r="G9">
         <v>3.399</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>12.129220999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>32</v>
       </c>
@@ -16198,6 +17243,9 @@
       <c r="C10">
         <v>0.64900000000000002</v>
       </c>
+      <c r="D10">
+        <v>2.310508</v>
+      </c>
       <c r="E10">
         <v>32</v>
       </c>
@@ -16207,8 +17255,11 @@
       <c r="G10">
         <v>2.76</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>9.5707269999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>48</v>
       </c>
@@ -16218,6 +17269,9 @@
       <c r="C11">
         <v>0.65100000000000002</v>
       </c>
+      <c r="D11">
+        <v>2.1547100000000001</v>
+      </c>
       <c r="E11">
         <v>48</v>
       </c>
@@ -16227,8 +17281,11 @@
       <c r="G11">
         <v>2.7610000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>7.9244919999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>64</v>
       </c>
@@ -16238,6 +17295,9 @@
       <c r="C12">
         <v>0.65300000000000002</v>
       </c>
+      <c r="D12">
+        <v>1.8771610000000001</v>
+      </c>
       <c r="E12">
         <v>64</v>
       </c>
@@ -16247,19 +17307,23 @@
       <c r="G12">
         <v>2.76</v>
       </c>
+      <c r="H12">
+        <v>7.1972329999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D59CA81-405D-412E-90F4-9035DC10537A}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16267,7 +17331,7 @@
     <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -16278,7 +17342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -16294,6 +17358,9 @@
       <c r="F2" t="s">
         <v>24</v>
       </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
@@ -16303,6 +17370,9 @@
       <c r="J2" t="s">
         <v>24</v>
       </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
       <c r="L2" t="s">
         <v>25</v>
       </c>
@@ -16312,8 +17382,11 @@
       <c r="N2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -16331,6 +17404,10 @@
         <f>$B$3 / Graphs!C3</f>
         <v>1.0029095643003099</v>
       </c>
+      <c r="G3">
+        <f>$B$4 / Graphs!D3</f>
+        <v>0.99699991795463661</v>
+      </c>
       <c r="H3">
         <v>1</v>
       </c>
@@ -16342,6 +17419,10 @@
         <f>$B$7 / Graphs!G3</f>
         <v>1.0030219251747716</v>
       </c>
+      <c r="K3">
+        <f>$B$8 / Graphs!H3</f>
+        <v>1.0094327428008203</v>
+      </c>
       <c r="L3">
         <v>8</v>
       </c>
@@ -16353,8 +17434,18 @@
         <f>$B$11 / Graphs!K3</f>
         <v>7.3845195493704443</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O3">
+        <f>$B$12 / Graphs!L3</f>
+        <v>3.8296174443546369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1">
+        <v>27.560312</v>
+      </c>
       <c r="D4">
         <v>2</v>
       </c>
@@ -16366,6 +17457,10 @@
         <f>$B$3 / Graphs!C4</f>
         <v>2.0041018177028449</v>
       </c>
+      <c r="G4">
+        <f>$B$4 / Graphs!D4</f>
+        <v>1.2617852429202105</v>
+      </c>
       <c r="H4">
         <v>2</v>
       </c>
@@ -16377,6 +17472,10 @@
         <f>$B$7 / Graphs!G4</f>
         <v>2.0048425158159819</v>
       </c>
+      <c r="K4">
+        <f>$B$8 / Graphs!H4</f>
+        <v>1.3212685653871361</v>
+      </c>
       <c r="L4">
         <v>16</v>
       </c>
@@ -16388,8 +17487,12 @@
         <f>$B$11 / Graphs!K4</f>
         <v>14.747538380095289</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O4">
+        <f>$B$12 / Graphs!L4</f>
+        <v>7.1491744404843462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -16404,6 +17507,10 @@
         <f>$B$3 / Graphs!C5</f>
         <v>3.8296352881953184</v>
       </c>
+      <c r="G5">
+        <f>$B$4 / Graphs!D5</f>
+        <v>2.1359099121217873</v>
+      </c>
       <c r="H5">
         <v>4</v>
       </c>
@@ -16415,6 +17522,10 @@
         <f>$B$7 / Graphs!G5</f>
         <v>3.8306350193639243</v>
       </c>
+      <c r="K5">
+        <f>$B$8 / Graphs!H5</f>
+        <v>2.1124372837412899</v>
+      </c>
       <c r="L5">
         <v>32</v>
       </c>
@@ -16426,8 +17537,12 @@
         <f>$B$11 / Graphs!K5</f>
         <v>23.727195298526532</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O5">
+        <f>$B$12 / Graphs!L5</f>
+        <v>11.704788685378515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -16445,6 +17560,10 @@
         <f>$B$3 / Graphs!C6</f>
         <v>7.3859907766990283</v>
       </c>
+      <c r="G6">
+        <f>$B$4 / Graphs!D6</f>
+        <v>3.5911489344402532</v>
+      </c>
       <c r="H6">
         <v>8</v>
       </c>
@@ -16456,6 +17575,10 @@
         <f>$B$7 / Graphs!G6</f>
         <v>7.3856411358750993</v>
       </c>
+      <c r="K6">
+        <f>$B$8 / Graphs!H6</f>
+        <v>3.7930485463063102</v>
+      </c>
       <c r="L6">
         <v>64</v>
       </c>
@@ -16467,8 +17590,12 @@
         <f>$B$11 / Graphs!K6</f>
         <v>23.727195298526532</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O6">
+        <f>$B$12 / Graphs!L6</f>
+        <v>15.431767725955957</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -16486,6 +17613,10 @@
         <f>$B$3 / Graphs!C7</f>
         <v>11.057515261627907</v>
       </c>
+      <c r="G7">
+        <f>$B$4 / Graphs!D7</f>
+        <v>5.3456335823020407</v>
+      </c>
       <c r="H7">
         <v>12</v>
       </c>
@@ -16497,8 +17628,18 @@
         <f>$B$7 / Graphs!G7</f>
         <v>11.075955548014932</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <f>$B$8 / Graphs!H7</f>
+        <v>5.6229545982478459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1">
+        <v>118.87842000000001</v>
+      </c>
       <c r="D8">
         <v>16</v>
       </c>
@@ -16510,6 +17651,10 @@
         <f>$B$3 / Graphs!C8</f>
         <v>14.615889529298752</v>
       </c>
+      <c r="G8">
+        <f>$B$4 / Graphs!D8</f>
+        <v>7.1745301855308332</v>
+      </c>
       <c r="H8">
         <v>16</v>
       </c>
@@ -16521,8 +17666,12 @@
         <f>$B$7 / Graphs!G8</f>
         <v>14.736271331828444</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <f>$B$8 / Graphs!H8</f>
+        <v>7.0988236505278159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -16537,6 +17686,10 @@
         <f>$B$3 / Graphs!C9</f>
         <v>19.138542138364777</v>
       </c>
+      <c r="G9">
+        <f>$B$4 / Graphs!D9</f>
+        <v>10.164294594507878</v>
+      </c>
       <c r="H9">
         <v>24</v>
       </c>
@@ -16548,8 +17701,12 @@
         <f>$B$7 / Graphs!G9</f>
         <v>19.206143571638719</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <f>$B$8 / Graphs!H9</f>
+        <v>9.8009938148542286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -16567,6 +17724,10 @@
         <f>$B$3 / Graphs!C10</f>
         <v>23.443976887519259</v>
       </c>
+      <c r="G10">
+        <f>$B$4 / Graphs!D10</f>
+        <v>11.928247813900667</v>
+      </c>
       <c r="H10">
         <v>32</v>
       </c>
@@ -16578,8 +17739,12 @@
         <f>$B$7 / Graphs!G10</f>
         <v>23.652783333333335</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K10">
+        <f>$B$8 / Graphs!H10</f>
+        <v>12.421043876813121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -16597,6 +17762,10 @@
         <f>$B$3 / Graphs!C11</f>
         <v>23.371952380952379</v>
       </c>
+      <c r="G11">
+        <f>$B$4 / Graphs!D11</f>
+        <v>12.790729146845747</v>
+      </c>
       <c r="H11">
         <v>48</v>
       </c>
@@ -16608,8 +17777,18 @@
         <f>$B$7 / Graphs!G11</f>
         <v>23.644216588192684</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <f>$B$8 / Graphs!H11</f>
+        <v>15.001393149239094</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>495.94460800000002</v>
+      </c>
       <c r="D12">
         <v>64</v>
       </c>
@@ -16621,6 +17800,10 @@
         <f>$B$3 / Graphs!C12</f>
         <v>23.300369065849921</v>
       </c>
+      <c r="G12">
+        <f>$B$4 / Graphs!D12</f>
+        <v>14.681911674065249</v>
+      </c>
       <c r="H12">
         <v>64</v>
       </c>
@@ -16631,6 +17814,65 @@
       <c r="J12">
         <f>$B$7 / Graphs!G12</f>
         <v>23.652783333333335</v>
+      </c>
+      <c r="K12">
+        <f>$B$8 / Graphs!H12</f>
+        <v>16.517239333504975</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -16643,7 +17885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B31564-144C-4844-89A5-1F6BF44FC46A}">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Swapped axes of graphs
</commit_message>
<xml_diff>
--- a/Go/results go.xlsx
+++ b/Go/results go.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxkb\OneDrive\Documents\Uni\Year 4\DPT\DPT-coursework\Go\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7685401B-2C3A-493F-AD69-4CD0E71F5802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721B3125-D7FF-4AD1-A8BE-F72B46F3781B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="5610" windowWidth="28800" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7660" yWindow="5550" windowWidth="28800" windowHeight="15450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results go" sheetId="1" r:id="rId1"/>
@@ -837,6 +837,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -870,45 +909,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.80270039400000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -960,6 +960,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -993,45 +1032,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.65300000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1083,6 +1083,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1116,45 +1155,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.8771610000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1221,7 +1221,7 @@
                   <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Median Runtime(s)</a:t>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="1000">
                   <a:effectLst/>
@@ -1340,9 +1340,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Number of Threads</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Median Runtime(s)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1612,6 +1617,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1645,45 +1689,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.377058415</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$E$3:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1735,6 +1740,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1768,45 +1812,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.76</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$E$3:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1858,6 +1863,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$H$3:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1891,45 +1935,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.1972329999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$E$3:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1996,7 +2001,7 @@
                   <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Median Runtime (s)</a:t>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="1000">
                   <a:effectLst/>
@@ -2115,14 +2120,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Median Runtime (s)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Threads</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2392,6 +2397,27 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$J$3:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2407,27 +2433,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14.205709568</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$I$3:$I$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2479,6 +2484,27 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$K$3:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2494,27 +2520,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>11.741</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$I$3:$I$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2566,6 +2571,27 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Graphs!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Graphs!$L$3:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2581,27 +2607,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>32.137900000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Graphs!$I$3:$I$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2668,7 +2673,7 @@
                   <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Median Runtime (s)</a:t>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="1000">
                   <a:effectLst/>
@@ -2787,9 +2792,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Number of Threads</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Median Runtime (s)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3059,6 +3069,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -3092,45 +3141,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>19.877058747276507</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$D$3:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3182,6 +3192,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -3215,45 +3264,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>23.300369065849921</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$D$3:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3305,6 +3315,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -3338,45 +3387,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>14.681911674065249</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$D$3:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3428,10 +3438,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Speedups!$A$16:$A$23</c:f>
+              <c:f>Speedups!$A$16:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3455,16 +3465,22 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Speedups!$A$16:$A$23</c:f>
+              <c:f>Speedups!$A$16:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3488,6 +3504,12 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3551,9 +3573,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Speedup</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3669,7 +3696,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Number of Threads</a:t>
+                  <a:t>Absolute Speedup</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3859,7 +3886,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> vs C+OpenMP Absolute Speedup</a:t>
+              <a:t> vs C+OpenMP vs Erlang Absolute Speedup</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -3940,6 +3967,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$I$3:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -3973,45 +4039,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>20.122262019266845</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$H$3:$H$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4063,6 +4090,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$J$3:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -4096,45 +4162,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>23.652783333333335</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$H$3:$H$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4186,6 +4213,45 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$K$3:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -4219,45 +4285,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>16.517239333504975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$H$3:$H$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4309,10 +4336,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Speedups!$A$16:$A$23</c:f>
+              <c:f>Speedups!$A$16:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4336,16 +4363,22 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Speedups!$A$16:$A$23</c:f>
+              <c:f>Speedups!$A$16:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4369,6 +4402,12 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4432,9 +4471,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Speedup</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4549,9 +4593,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Number of Threads</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Absolute Speedup</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4740,7 +4789,17 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> vs C+OpenMP Absolute Speedup</a:t>
+              <a:t> vs C+OpenMP</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> vs Erlang</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Absolute Speedup</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -4821,6 +4880,27 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$L$3:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$M$3:$M$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -4836,27 +4916,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20.733962046041459</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$L$3:$L$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4908,6 +4967,27 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$L$3:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$N$3:$N$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -4923,27 +5003,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>23.727195298526532</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$L$3:$L$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4995,6 +5054,27 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Speedups!$L$3:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Speedups!$O$3:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -5010,27 +5090,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15.431767725955957</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Speedups!$L$3:$L$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5082,42 +5141,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(Speedups!$A$16,Speedups!$A$19,Speedups!$A$21,Speedups!$A$23)</c:f>
+              <c:f>(Speedups!$A$19,Speedups!$A$21,Speedups!$A$23,Speedups!$A$25)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Speedups!$A$16,Speedups!$A$19,Speedups!$A$21,Speedups!$A$23)</c:f>
+              <c:f>(Speedups!$A$19,Speedups!$A$21,Speedups!$A$23,Speedups!$A$25)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5181,9 +5240,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Speedup</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5298,9 +5362,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Number of Threads</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Absolute Speedup</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -16948,7 +17017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2401614-BA96-48EB-BC57-655DFAADC499}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y37" sqref="Y37"/>
     </sheetView>
   </sheetViews>
@@ -17322,8 +17391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D59CA81-405D-412E-90F4-9035DC10537A}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>